<commit_message>
chore: add source code
</commit_message>
<xml_diff>
--- a/planilha_dados.xlsx
+++ b/planilha_dados.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
-  <si>
-    <t xml:space="preserve">tipo_contrato</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t xml:space="preserve">nome_contratada</t>
   </si>
@@ -46,9 +43,6 @@
     <t xml:space="preserve">nome_assinatura2</t>
   </si>
   <si>
-    <t xml:space="preserve">VENDA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nome da Primeira empresa</t>
   </si>
   <si>
@@ -65,9 +59,6 @@
   </si>
   <si>
     <t xml:space="preserve">Seu João – Contratante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SERVIÇO</t>
   </si>
   <si>
     <t xml:space="preserve">Empresa de serviços</t>
@@ -174,7 +165,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,18 +175,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -224,140 +207,127 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="26.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="29.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.67"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="B2" s="4" t="n">
+        <v>123123123123123</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="n">
-        <v>123123123123123</v>
-      </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="6" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="B3" s="4" t="n">
+        <v>777777777777777</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="n">
-        <v>777777777777777</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="5"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="7"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>